<commit_message>
Database Update, Dar Startup Update
</commit_message>
<xml_diff>
--- a/pyArch.extension/pyArch.tab/Doors.panel/Door Design Database.xlsx
+++ b/pyArch.extension/pyArch.tab/Doors.panel/Door Design Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkumar2\Desktop\pyRevit Toolbars\01_Tools\pyArch\pyArch.extension\pyArch.tab\Doors.panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEBAF5F-A68F-497A-8876-C1B7AF96C39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65D78AD-5E37-4ADE-A9DE-AEAAB54FA372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{43157EDF-9DF6-4BE5-989B-599A16B6E66A}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="136">
   <si>
     <t>ROOM TYPE</t>
   </si>
@@ -383,9 +383,6 @@
     <t>AHU</t>
   </si>
   <si>
-    <t>HABITABLE ROOM</t>
-  </si>
-  <si>
     <t>SMALL STORAGE</t>
   </si>
   <si>
@@ -417,6 +414,45 @@
   </si>
   <si>
     <t>GARBAGE ROOM</t>
+  </si>
+  <si>
+    <t>FIRE TANK</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>HABITABLE ROOM (FOH)</t>
+  </si>
+  <si>
+    <t>HABITABLE ROOM (BOH)</t>
+  </si>
+  <si>
+    <t>RETAIL</t>
+  </si>
+  <si>
+    <t>F&amp;B</t>
+  </si>
+  <si>
+    <t>GENERATOR ROOM</t>
+  </si>
+  <si>
+    <t>EXHBITION SPACES</t>
+  </si>
+  <si>
+    <t>MEETING ROOM</t>
+  </si>
+  <si>
+    <t>LOBBY (BOH)</t>
+  </si>
+  <si>
+    <t>LOBBY (FOH)</t>
+  </si>
+  <si>
+    <t>ABLUTION ROOM</t>
+  </si>
+  <si>
+    <t>LOUNGE</t>
   </si>
 </sst>
 </file>
@@ -1236,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAA63AA-A98E-4DCB-A01B-5B1BE0C8ED98}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,7 +1328,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -1327,7 +1363,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1362,7 +1398,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1397,13 +1433,11 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="D5" s="1">
         <v>2200</v>
@@ -1412,22 +1446,22 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1438,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="1">
         <v>2200</v>
@@ -1467,7 +1501,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1488,7 +1522,7 @@
         <v>78</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>13</v>
@@ -1497,12 +1531,12 @@
         <v>45</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -1572,22 +1606,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="D10" s="1">
-        <v>1900</v>
+        <v>2200</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>78</v>
@@ -1596,7 +1630,7 @@
         <v>24</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>45</v>
@@ -1607,22 +1641,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>1100</v>
+        <v>600</v>
       </c>
       <c r="D11" s="1">
-        <v>2200</v>
+        <v>1900</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>78</v>
@@ -1631,7 +1665,7 @@
         <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>45</v>
@@ -1642,22 +1676,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="D12" s="1">
-        <v>1800</v>
+        <v>2200</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>78</v>
@@ -1666,7 +1700,7 @@
         <v>24</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>45</v>
@@ -1677,7 +1711,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1692,16 +1726,16 @@
         <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>45</v>
@@ -1712,16 +1746,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="D14" s="1">
-        <v>2200</v>
+        <v>1800</v>
       </c>
       <c r="E14" s="1">
         <v>10</v>
@@ -1747,13 +1781,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="D15" s="1">
         <v>2200</v>
@@ -1762,33 +1796,33 @@
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="D16" s="1">
         <v>2200</v>
@@ -1817,7 +1851,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1829,30 +1863,30 @@
         <v>2200</v>
       </c>
       <c r="E17" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -1864,36 +1898,36 @@
         <v>2200</v>
       </c>
       <c r="E18" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="D19" s="1">
         <v>2200</v>
@@ -1922,7 +1956,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -1957,16 +1991,16 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>2400</v>
+        <v>1000</v>
       </c>
       <c r="D21" s="1">
-        <v>3000</v>
+        <v>2200</v>
       </c>
       <c r="E21" s="1">
         <v>10</v>
@@ -1975,7 +2009,7 @@
         <v>31</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>24</v>
@@ -1992,13 +2026,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1">
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="D22" s="1">
         <v>2200</v>
@@ -2027,13 +2061,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1">
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="D23" s="1">
         <v>2200</v>
@@ -2042,237 +2076,215 @@
         <v>10</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>133</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
       </c>
       <c r="C24" s="1">
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="D24" s="1">
-        <v>3000</v>
+        <v>2200</v>
       </c>
       <c r="E24" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="1">
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="D25" s="1">
-        <v>2700</v>
+        <v>2200</v>
       </c>
       <c r="E25" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
       </c>
       <c r="C26" s="1">
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="D26" s="1">
-        <v>2700</v>
+        <v>2200</v>
       </c>
       <c r="E26" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
       <c r="C27" s="1">
-        <v>900</v>
+        <v>1200</v>
       </c>
       <c r="D27" s="1">
         <v>2200</v>
       </c>
       <c r="E27" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="D28" s="1">
         <v>2200</v>
       </c>
       <c r="E28" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>45</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1800</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2200</v>
-      </c>
-      <c r="E29" s="1">
-        <v>10</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -2307,13 +2319,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" s="1">
-        <v>900</v>
+        <v>2400</v>
       </c>
       <c r="D31" s="1">
         <v>2200</v>
@@ -2342,16 +2354,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1">
         <v>2</v>
       </c>
       <c r="C32" s="1">
-        <v>1400</v>
+        <v>2400</v>
       </c>
       <c r="D32" s="1">
-        <v>2200</v>
+        <v>3000</v>
       </c>
       <c r="E32" s="1">
         <v>10</v>
@@ -2360,7 +2372,7 @@
         <v>31</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>24</v>
@@ -2377,13 +2389,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="1">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="D33" s="1">
         <v>2200</v>
@@ -2412,13 +2424,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="B34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="D34" s="1">
         <v>2200</v>
@@ -2447,16 +2459,16 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="B35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35" s="1">
-        <v>900</v>
+        <v>2000</v>
       </c>
       <c r="D35" s="1">
-        <v>2200</v>
+        <v>3000</v>
       </c>
       <c r="E35" s="1">
         <v>10</v>
@@ -2482,16 +2494,16 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1">
         <v>2</v>
       </c>
       <c r="C36" s="1">
-        <v>2400</v>
+        <v>1400</v>
       </c>
       <c r="D36" s="1">
-        <v>2200</v>
+        <v>2700</v>
       </c>
       <c r="E36" s="1">
         <v>10</v>
@@ -2517,16 +2529,16 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>111</v>
+        <v>8</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" s="1">
-        <v>3200</v>
+        <v>1400</v>
       </c>
       <c r="D37" s="1">
-        <v>3200</v>
+        <v>2700</v>
       </c>
       <c r="E37" s="1">
         <v>10</v>
@@ -2551,43 +2563,21 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1200</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2200</v>
-      </c>
-      <c r="E38" s="1">
-        <v>10</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -2602,42 +2592,497 @@
         <v>10</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E40" s="1">
+        <v>10</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1800</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E41" s="1">
+        <v>10</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1">
+        <v>900</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E42" s="1">
+        <v>10</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1">
+        <v>900</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E43" s="1">
+        <v>10</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1400</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E44" s="1">
+        <v>10</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1400</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E45" s="1">
+        <v>10</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1400</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E46" s="1">
+        <v>10</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1">
+        <v>900</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E48" s="1">
+        <v>10</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2400</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E49" s="1">
+        <v>10</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3200</v>
+      </c>
+      <c r="D50" s="1">
+        <v>3200</v>
+      </c>
+      <c r="E50" s="1">
+        <v>10</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D51" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E51" s="1">
+        <v>10</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>900</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E52" s="1">
+        <v>10</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="1" t="s">
+      <c r="G52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="J52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1600</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2200</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Door Nib Ownership Check
</commit_message>
<xml_diff>
--- a/pyArch.extension/pyArch.tab/Doors.panel/Door Design Database.xlsx
+++ b/pyArch.extension/pyArch.tab/Doors.panel/Door Design Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkumar2\Desktop\pyRevit Toolbars\01_Tools\pyArch\pyArch.extension\pyArch.tab\Doors.panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D7ED11-DB2F-4814-8FF4-227740EB6BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F780DDCF-27CE-47F1-BBA8-5772B930FF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-15020" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{43157EDF-9DF6-4BE5-989B-599A16B6E66A}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="135">
   <si>
     <t>ROOM TYPE</t>
   </si>
@@ -417,9 +417,6 @@
   </si>
   <si>
     <t>FIRE TANK</t>
-  </si>
-  <si>
-    <t>10</t>
   </si>
   <si>
     <t>HABITABLE ROOM (FOH)</t>
@@ -544,7 +541,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -572,9 +569,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -934,228 +928,228 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>3</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="13">
+      <c r="B17" s="12">
         <v>4</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="B19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1275,7 +1269,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1278,7 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="11" customWidth="1"/>
     <col min="6" max="7" width="25.28515625" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" customWidth="1"/>
     <col min="9" max="11" width="19.28515625" customWidth="1"/>
@@ -1398,7 +1392,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -1433,7 +1427,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -1711,7 +1705,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1886,7 +1880,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -2061,7 +2055,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
@@ -2096,7 +2090,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
@@ -2131,7 +2125,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
@@ -2166,7 +2160,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
@@ -2201,7 +2195,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -2236,7 +2230,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -2306,7 +2300,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="1">
         <v>2</v>
@@ -3017,8 +3011,8 @@
       <c r="D50" s="1">
         <v>2200</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>124</v>
+      <c r="E50" s="1">
+        <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>31</v>

</xml_diff>